<commit_message>
Deneme commit message for changes made
</commit_message>
<xml_diff>
--- a/Yeni Veri/Q-1-calibrated.xlsx
+++ b/Yeni Veri/Q-1-calibrated.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Calibrated Results" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Human Reference (5 samples)" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Calibrated Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Human Reference (5 samples)" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -501,7 +501,7 @@
         <v>18</v>
       </c>
       <c r="H2" t="n">
-        <v>18.83539541159658</v>
+        <v>18.83539263274327</v>
       </c>
     </row>
     <row r="3">
@@ -529,7 +529,7 @@
         <v>16</v>
       </c>
       <c r="H3" t="n">
-        <v>16.1336439950068</v>
+        <v>16.13368254854908</v>
       </c>
     </row>
     <row r="4">
@@ -557,7 +557,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="n">
-        <v>13.60585718298769</v>
+        <v>13.60588575162473</v>
       </c>
     </row>
     <row r="5">
@@ -585,7 +585,7 @@
         <v>17</v>
       </c>
       <c r="H5" t="n">
-        <v>17.27767291025862</v>
+        <v>17.27770529281258</v>
       </c>
     </row>
     <row r="6">
@@ -613,7 +613,7 @@
         <v>16</v>
       </c>
       <c r="H6" t="n">
-        <v>17.2973031848559</v>
+        <v>17.29730638024663</v>
       </c>
     </row>
     <row r="7">
@@ -641,7 +641,7 @@
         <v>18</v>
       </c>
       <c r="H7" t="n">
-        <v>17.98112660618836</v>
+        <v>17.98114245281742</v>
       </c>
     </row>
     <row r="8">
@@ -669,7 +669,7 @@
         <v>16</v>
       </c>
       <c r="H8" t="n">
-        <v>16.36913203153326</v>
+        <v>16.36918542493153</v>
       </c>
     </row>
     <row r="9">
@@ -697,7 +697,7 @@
         <v>17</v>
       </c>
       <c r="H9" t="n">
-        <v>17.27767291025862</v>
+        <v>17.27770529281258</v>
       </c>
     </row>
     <row r="10">
@@ -725,7 +725,7 @@
         <v>16</v>
       </c>
       <c r="H10" t="n">
-        <v>16.61772070851246</v>
+        <v>16.61771873969076</v>
       </c>
     </row>
     <row r="11">
@@ -753,7 +753,7 @@
         <v>16</v>
       </c>
       <c r="H11" t="n">
-        <v>15.65914870145899</v>
+        <v>15.65917761586943</v>
       </c>
     </row>
     <row r="12">
@@ -781,7 +781,7 @@
         <v>16</v>
       </c>
       <c r="H12" t="n">
-        <v>16.07284228754513</v>
+        <v>16.07284221153662</v>
       </c>
     </row>
     <row r="13">
@@ -809,7 +809,7 @@
         <v>16</v>
       </c>
       <c r="H13" t="n">
-        <v>16.38223267198601</v>
+        <v>16.38221586330832</v>
       </c>
     </row>
     <row r="14">
@@ -837,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="H14" t="n">
-        <v>16.13292227051268</v>
+        <v>16.13293329644894</v>
       </c>
     </row>
     <row r="15">
@@ -865,7 +865,7 @@
         <v>15</v>
       </c>
       <c r="H15" t="n">
-        <v>16.45308323408712</v>
+        <v>16.45312602929282</v>
       </c>
     </row>
     <row r="16">
@@ -893,7 +893,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="n">
-        <v>15.78308217770153</v>
+        <v>15.78306964719897</v>
       </c>
     </row>
     <row r="17">
@@ -921,7 +921,7 @@
         <v>14</v>
       </c>
       <c r="H17" t="n">
-        <v>14.84414044524534</v>
+        <v>14.84412961081168</v>
       </c>
     </row>
     <row r="18">
@@ -949,7 +949,7 @@
         <v>15</v>
       </c>
       <c r="H18" t="n">
-        <v>16.18367512333492</v>
+        <v>16.18370380448937</v>
       </c>
     </row>
     <row r="19">
@@ -977,7 +977,7 @@
         <v>16</v>
       </c>
       <c r="H19" t="n">
-        <v>17.12261685579112</v>
+        <v>17.12264384087666</v>
       </c>
     </row>
     <row r="20">
@@ -1005,7 +1005,7 @@
         <v>16</v>
       </c>
       <c r="H20" t="n">
-        <v>16.51693672736211</v>
+        <v>16.51692697571005</v>
       </c>
     </row>
     <row r="21">
@@ -1033,7 +1033,7 @@
         <v>15</v>
       </c>
       <c r="H21" t="n">
-        <v>15.39978944534623</v>
+        <v>15.39982522003801</v>
       </c>
     </row>
     <row r="22">
@@ -1061,7 +1061,7 @@
         <v>15</v>
       </c>
       <c r="H22" t="n">
-        <v>14.75060782273363</v>
+        <v>14.75065774798837</v>
       </c>
     </row>
     <row r="23">
@@ -1089,7 +1089,7 @@
         <v>15</v>
       </c>
       <c r="H23" t="n">
-        <v>17.32045267994808</v>
+        <v>17.32040664759545</v>
       </c>
     </row>
     <row r="24">
@@ -1117,7 +1117,7 @@
         <v>18</v>
       </c>
       <c r="H24" t="n">
-        <v>18.12541208152231</v>
+        <v>18.12538482368117</v>
       </c>
     </row>
     <row r="25">
@@ -1145,7 +1145,7 @@
         <v>15</v>
       </c>
       <c r="H25" t="n">
-        <v>16.03938964800097</v>
+        <v>16.03946143362563</v>
       </c>
     </row>
     <row r="26">
@@ -1173,7 +1173,7 @@
         <v>17</v>
       </c>
       <c r="H26" t="n">
-        <v>17.62098336892524</v>
+        <v>17.62099829300529</v>
       </c>
     </row>
     <row r="27">
@@ -1201,7 +1201,7 @@
         <v>17</v>
       </c>
       <c r="H27" t="n">
-        <v>17.36467589862579</v>
+        <v>17.36460650657863</v>
       </c>
     </row>
     <row r="28">
@@ -1229,7 +1229,7 @@
         <v>16</v>
       </c>
       <c r="H28" t="n">
-        <v>15.92503759171628</v>
+        <v>15.9251006607581</v>
       </c>
     </row>
     <row r="29">
@@ -1257,7 +1257,7 @@
         <v>18</v>
       </c>
       <c r="H29" t="n">
-        <v>18.9128169800059</v>
+        <v>18.9127625880473</v>
       </c>
     </row>
     <row r="30">
@@ -1285,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="H30" t="n">
-        <v>17.41165524114059</v>
+        <v>17.41166715311416</v>
       </c>
     </row>
     <row r="31">
@@ -1313,7 +1313,7 @@
         <v>18</v>
       </c>
       <c r="H31" t="n">
-        <v>18.42522104600534</v>
+        <v>18.42522721699085</v>
       </c>
     </row>
     <row r="32">
@@ -1341,7 +1341,7 @@
         <v>13</v>
       </c>
       <c r="H32" t="n">
-        <v>13.65661003580993</v>
+        <v>13.65665625966516</v>
       </c>
     </row>
     <row r="33">
@@ -1369,7 +1369,7 @@
         <v>15</v>
       </c>
       <c r="H33" t="n">
-        <v>16.6277695631519</v>
+        <v>16.62778856866279</v>
       </c>
     </row>
     <row r="34">
@@ -1397,7 +1397,7 @@
         <v>16</v>
       </c>
       <c r="H34" t="n">
-        <v>16.29522968361884</v>
+        <v>16.29531464954227</v>
       </c>
     </row>
     <row r="35">
@@ -1425,7 +1425,7 @@
         <v>18</v>
       </c>
       <c r="H35" t="n">
-        <v>19.61928108958527</v>
+        <v>19.61927121719463</v>
       </c>
     </row>
     <row r="36">
@@ -1453,7 +1453,7 @@
         <v>16</v>
       </c>
       <c r="H36" t="n">
-        <v>16.61772070851246</v>
+        <v>16.61771873969076</v>
       </c>
     </row>
     <row r="37">
@@ -1481,7 +1481,7 @@
         <v>16</v>
       </c>
       <c r="H37" t="n">
-        <v>17.33122325908164</v>
+        <v>17.33122572866764</v>
       </c>
     </row>
     <row r="38">
@@ -1509,7 +1509,7 @@
         <v>16</v>
       </c>
       <c r="H38" t="n">
-        <v>16.85320874503892</v>
+        <v>16.85322161607321</v>
       </c>
     </row>
     <row r="39">
@@ -1537,7 +1537,7 @@
         <v>17</v>
       </c>
       <c r="H39" t="n">
-        <v>18.41445046687178</v>
+        <v>18.41440813591867</v>
       </c>
     </row>
     <row r="40">
@@ -1589,7 +1589,7 @@
         <v>15</v>
       </c>
       <c r="H41" t="n">
-        <v>15.75268132397069</v>
+        <v>15.75264947869274</v>
       </c>
     </row>
     <row r="42">
@@ -1617,7 +1617,7 @@
         <v>18</v>
       </c>
       <c r="H42" t="n">
-        <v>18.83539541159658</v>
+        <v>18.83539263274327</v>
       </c>
     </row>
     <row r="43">
@@ -1645,7 +1645,7 @@
         <v>17</v>
       </c>
       <c r="H43" t="n">
-        <v>16.88059918512013</v>
+        <v>16.88057031543696</v>
       </c>
     </row>
     <row r="44">
@@ -1673,7 +1673,7 @@
         <v>14</v>
       </c>
       <c r="H44" t="n">
-        <v>15.44982057367434</v>
+        <v>15.44984647597829</v>
       </c>
     </row>
     <row r="45">
@@ -1701,7 +1701,7 @@
         <v>15</v>
       </c>
       <c r="H45" t="n">
-        <v>15.81348303143237</v>
+        <v>15.8134898157052</v>
       </c>
     </row>
     <row r="46">
@@ -1729,7 +1729,7 @@
         <v>14</v>
       </c>
       <c r="H46" t="n">
-        <v>14.5216494203517</v>
+        <v>14.52172552066319</v>
       </c>
     </row>
     <row r="47">
@@ -1757,7 +1757,7 @@
         <v>16</v>
       </c>
       <c r="H47" t="n">
-        <v>15.86423588425461</v>
+        <v>15.86426032374564</v>
       </c>
     </row>
     <row r="48">
@@ -1785,7 +1785,7 @@
         <v>16</v>
       </c>
       <c r="H48" t="n">
-        <v>16.67852241597414</v>
+        <v>16.67855907670323</v>
       </c>
     </row>
     <row r="49">
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
       <c r="H49" t="n">
-        <v>17.41237696563472</v>
+        <v>17.41241640521431</v>
       </c>
     </row>
     <row r="50">
@@ -1841,7 +1841,7 @@
         <v>14</v>
       </c>
       <c r="H50" t="n">
-        <v>14.18185818217998</v>
+        <v>14.18193170038525</v>
       </c>
     </row>
     <row r="51">
@@ -1869,7 +1869,7 @@
         <v>15</v>
       </c>
       <c r="H51" t="n">
-        <v>14.95569500552925</v>
+        <v>14.95574045586458</v>
       </c>
     </row>
     <row r="52">
@@ -1897,7 +1897,7 @@
         <v>17</v>
       </c>
       <c r="H52" t="n">
-        <v>16.87707996462523</v>
+        <v>16.87707113552218</v>
       </c>
     </row>
     <row r="53">
@@ -1925,7 +1925,7 @@
         <v>17</v>
       </c>
       <c r="H53" t="n">
-        <v>18.04425837496922</v>
+        <v>18.0441941471345</v>
       </c>
     </row>
     <row r="54">
@@ -1953,7 +1953,7 @@
         <v>14</v>
       </c>
       <c r="H54" t="n">
-        <v>15.8235318860718</v>
+        <v>15.82355964467723</v>
       </c>
     </row>
     <row r="55">
@@ -1981,7 +1981,7 @@
         <v>15</v>
       </c>
       <c r="H55" t="n">
-        <v>15.78308217770153</v>
+        <v>15.78306964719897</v>
       </c>
     </row>
     <row r="56">
@@ -2009,7 +2009,7 @@
         <v>16</v>
       </c>
       <c r="H56" t="n">
-        <v>16.82632711180299</v>
+        <v>16.82630062748175</v>
       </c>
     </row>
     <row r="57">
@@ -2037,7 +2037,7 @@
         <v>16</v>
       </c>
       <c r="H57" t="n">
-        <v>16.72202391015773</v>
+        <v>16.72200968358626</v>
       </c>
     </row>
     <row r="58">
@@ -2065,7 +2065,7 @@
         <v>17</v>
       </c>
       <c r="H58" t="n">
-        <v>18.34054811895736</v>
+        <v>18.34053736052941</v>
       </c>
     </row>
     <row r="59">
@@ -2117,7 +2117,7 @@
         <v>15</v>
       </c>
       <c r="H60" t="n">
-        <v>16.15327426960408</v>
+        <v>16.15328363598313</v>
       </c>
     </row>
     <row r="61">
@@ -2145,7 +2145,7 @@
         <v>17</v>
       </c>
       <c r="H61" t="n">
-        <v>16.67199278182961</v>
+        <v>16.67198842764597</v>
       </c>
     </row>
     <row r="62">
@@ -2173,7 +2173,7 @@
         <v>15</v>
       </c>
       <c r="H62" t="n">
-        <v>15.94818708680846</v>
+        <v>15.94820092810693</v>
       </c>
     </row>
     <row r="63">
@@ -2201,7 +2201,7 @@
         <v>17</v>
       </c>
       <c r="H63" t="n">
-        <v>17.48627931354914</v>
+        <v>17.48628718060356</v>
       </c>
     </row>
     <row r="64">
@@ -2253,7 +2253,7 @@
         <v>17</v>
       </c>
       <c r="H65" t="n">
-        <v>17.66096564261392</v>
+        <v>17.66094971997354</v>
       </c>
     </row>
     <row r="66">
@@ -2281,7 +2281,7 @@
         <v>17</v>
       </c>
       <c r="H66" t="n">
-        <v>17.42547760608747</v>
+        <v>17.4254468435911</v>
       </c>
     </row>
     <row r="67">
@@ -2309,7 +2309,7 @@
         <v>19</v>
       </c>
       <c r="H67" t="n">
-        <v>19.61275145544074</v>
+        <v>19.61270056813738</v>
       </c>
     </row>
     <row r="68">
@@ -2361,7 +2361,7 @@
         <v>17</v>
       </c>
       <c r="H69" t="n">
-        <v>17.97035602705481</v>
+        <v>17.97032337174524</v>
       </c>
     </row>
     <row r="70">
@@ -2389,7 +2389,7 @@
         <v>18</v>
       </c>
       <c r="H70" t="n">
-        <v>18.36441933854366</v>
+        <v>18.36438687997839</v>
       </c>
     </row>
     <row r="71">
@@ -2417,7 +2417,7 @@
         <v>17</v>
       </c>
       <c r="H71" t="n">
-        <v>17.38197611190388</v>
+        <v>17.38199623670807</v>
       </c>
     </row>
     <row r="72">
@@ -2445,7 +2445,7 @@
         <v>17</v>
       </c>
       <c r="H72" t="n">
-        <v>16.77629598347487</v>
+        <v>16.77627937154146</v>
       </c>
     </row>
     <row r="73">
@@ -2473,7 +2473,7 @@
         <v>15</v>
       </c>
       <c r="H73" t="n">
-        <v>16.15327426960408</v>
+        <v>16.15328363598313</v>
       </c>
     </row>
     <row r="74">
@@ -2501,7 +2501,7 @@
         <v>16</v>
       </c>
       <c r="H74" t="n">
-        <v>17.432007240232</v>
+        <v>17.43201749264836</v>
       </c>
     </row>
     <row r="75">
@@ -2529,7 +2529,7 @@
         <v>17</v>
       </c>
       <c r="H75" t="n">
-        <v>17.24727205652778</v>
+        <v>17.24728512430634</v>
       </c>
     </row>
     <row r="76">
@@ -2557,7 +2557,7 @@
         <v>18</v>
       </c>
       <c r="H76" t="n">
-        <v>18.73461143044622</v>
+        <v>18.73460086876256</v>
       </c>
     </row>
     <row r="77">
@@ -2585,7 +2585,7 @@
         <v>14</v>
       </c>
       <c r="H77" t="n">
-        <v>15.92783508771706</v>
+        <v>15.92785058857272</v>
       </c>
     </row>
     <row r="78">
@@ -2613,7 +2613,7 @@
         <v>14</v>
       </c>
       <c r="H78" t="n">
-        <v>14.87454129897617</v>
+        <v>14.87454977931792</v>
       </c>
     </row>
     <row r="79">
@@ -2641,7 +2641,7 @@
         <v>13</v>
       </c>
       <c r="H79" t="n">
-        <v>13.68349166904587</v>
+        <v>13.68357724825662</v>
       </c>
     </row>
     <row r="80">
@@ -2669,7 +2669,7 @@
         <v>15</v>
       </c>
       <c r="H80" t="n">
-        <v>15.36938859161539</v>
+        <v>15.36940505153178</v>
       </c>
     </row>
     <row r="81">
@@ -2721,7 +2721,7 @@
         <v>15</v>
       </c>
       <c r="H82" t="n">
-        <v>15.93508644635571</v>
+        <v>15.93517048973013</v>
       </c>
     </row>
     <row r="83">
@@ -2749,7 +2749,7 @@
         <v>16</v>
       </c>
       <c r="H83" t="n">
-        <v>16.62123992900737</v>
+        <v>16.62121791960553</v>
       </c>
     </row>
     <row r="84">
@@ -2777,7 +2777,7 @@
         <v>19</v>
       </c>
       <c r="H84" t="n">
-        <v>19.56924996125715</v>
+        <v>19.56924996125434</v>
       </c>
     </row>
     <row r="85">
@@ -2805,7 +2805,7 @@
         <v>17</v>
       </c>
       <c r="H85" t="n">
-        <v>17.01178402000133</v>
+        <v>17.0117822479239</v>
       </c>
     </row>
     <row r="86">
@@ -2833,7 +2833,7 @@
         <v>17</v>
       </c>
       <c r="H86" t="n">
-        <v>17.66096564261392</v>
+        <v>17.66094971997354</v>
       </c>
     </row>
     <row r="87">
@@ -2861,7 +2861,7 @@
         <v>18</v>
       </c>
       <c r="H87" t="n">
-        <v>18.49560417342486</v>
+        <v>18.49559881246534</v>
       </c>
     </row>
     <row r="88">
@@ -2889,7 +2889,7 @@
         <v>18</v>
       </c>
       <c r="H88" t="n">
-        <v>19.0440018148871</v>
+        <v>19.04397452053426</v>
       </c>
     </row>
     <row r="89">
@@ -2917,7 +2917,7 @@
         <v>17</v>
       </c>
       <c r="H89" t="n">
-        <v>18.84192504574111</v>
+        <v>18.84196328180053</v>
       </c>
     </row>
     <row r="90">
@@ -2945,7 +2945,7 @@
         <v>18</v>
       </c>
       <c r="H90" t="n">
-        <v>18.43480246596318</v>
+        <v>18.43475847545287</v>
       </c>
     </row>
     <row r="91">
@@ -2973,7 +2973,7 @@
         <v>14</v>
       </c>
       <c r="H91" t="n">
-        <v>14.5251686408466</v>
+        <v>14.52522470057796</v>
       </c>
     </row>
     <row r="92">
@@ -3001,7 +3001,7 @@
         <v>16</v>
       </c>
       <c r="H92" t="n">
-        <v>16.79592625807215</v>
+        <v>16.79588045897551</v>
       </c>
     </row>
     <row r="93">
@@ -3029,7 +3029,7 @@
         <v>14</v>
       </c>
       <c r="H93" t="n">
-        <v>16.02861906886742</v>
+        <v>16.02864235255344</v>
       </c>
     </row>
     <row r="94">
@@ -3057,7 +3057,7 @@
         <v>17</v>
       </c>
       <c r="H94" t="n">
-        <v>17.86605282540954</v>
+        <v>17.86603242784975</v>
       </c>
     </row>
     <row r="95">
@@ -3085,7 +3085,7 @@
         <v>18</v>
       </c>
       <c r="H95" t="n">
-        <v>18.45562189973617</v>
+        <v>18.45564738549708</v>
       </c>
     </row>
     <row r="96">
@@ -3113,7 +3113,7 @@
         <v>15</v>
       </c>
       <c r="H96" t="n">
-        <v>15.29900546419587</v>
+        <v>15.29903345605729</v>
       </c>
     </row>
     <row r="97">
@@ -3141,7 +3141,7 @@
         <v>14</v>
       </c>
       <c r="H97" t="n">
-        <v>15.28471566456741</v>
+        <v>15.28471519507034</v>
       </c>
     </row>
     <row r="98">
@@ -3169,7 +3169,7 @@
         <v>17</v>
       </c>
       <c r="H98" t="n">
-        <v>16.67199278182961</v>
+        <v>16.67198842764597</v>
       </c>
     </row>
     <row r="99">
@@ -3197,7 +3197,7 @@
         <v>17</v>
       </c>
       <c r="H99" t="n">
-        <v>17.55666244096866</v>
+        <v>17.55665877607805</v>
       </c>
     </row>
     <row r="100">
@@ -3225,7 +3225,7 @@
         <v>15</v>
       </c>
       <c r="H100" t="n">
-        <v>16.01857021422799</v>
+        <v>16.01857252358141</v>
       </c>
     </row>
     <row r="101">
@@ -3253,7 +3253,7 @@
         <v>16</v>
       </c>
       <c r="H101" t="n">
-        <v>16.62123992900737</v>
+        <v>16.62121791960553</v>
       </c>
     </row>
     <row r="102">
@@ -3281,7 +3281,7 @@
         <v>16</v>
       </c>
       <c r="H102" t="n">
-        <v>16.85672796553382</v>
+        <v>16.85672079598798</v>
       </c>
     </row>
     <row r="103">
@@ -3333,7 +3333,7 @@
         <v>17</v>
       </c>
       <c r="H104" t="n">
-        <v>17.69488571683966</v>
+        <v>17.69486906839455</v>
       </c>
     </row>
     <row r="105">
@@ -3361,7 +3361,7 @@
         <v>18</v>
       </c>
       <c r="H105" t="n">
-        <v>18.36441933854366</v>
+        <v>18.36438687997839</v>
       </c>
     </row>
     <row r="106">
@@ -3389,7 +3389,7 @@
         <v>14</v>
       </c>
       <c r="H106" t="n">
-        <v>14.12105647471831</v>
+        <v>14.12109136337278</v>
       </c>
     </row>
     <row r="107">
@@ -3417,7 +3417,7 @@
         <v>14</v>
       </c>
       <c r="H107" t="n">
-        <v>14.91804279315976</v>
+        <v>14.91800038620094</v>
       </c>
     </row>
     <row r="108">
@@ -3445,7 +3445,7 @@
         <v>15</v>
       </c>
       <c r="H108" t="n">
-        <v>16.32796059866887</v>
+        <v>16.32794617535311</v>
       </c>
     </row>
     <row r="109">
@@ -3473,7 +3473,7 @@
         <v>16</v>
       </c>
       <c r="H109" t="n">
-        <v>16.79240703757725</v>
+        <v>16.79238127906074</v>
       </c>
     </row>
     <row r="110">
@@ -3501,7 +3501,7 @@
         <v>17</v>
       </c>
       <c r="H110" t="n">
-        <v>17.24727205652778</v>
+        <v>17.24728512430634</v>
       </c>
     </row>
     <row r="111">
@@ -3529,7 +3529,7 @@
         <v>16</v>
       </c>
       <c r="H111" t="n">
-        <v>17.66749527675845</v>
+        <v>17.6675203690308</v>
       </c>
     </row>
     <row r="112">
@@ -3557,7 +3557,7 @@
         <v>16</v>
       </c>
       <c r="H112" t="n">
-        <v>16.17714548919039</v>
+        <v>16.17713315543211</v>
       </c>
     </row>
     <row r="113">
@@ -3585,7 +3585,7 @@
         <v>15</v>
       </c>
       <c r="H113" t="n">
-        <v>16.52698558200154</v>
+        <v>16.52699680468207</v>
       </c>
     </row>
     <row r="114">
@@ -3613,7 +3613,7 @@
         <v>18</v>
       </c>
       <c r="H114" t="n">
-        <v>18.42522104600534</v>
+        <v>18.42522721699085</v>
       </c>
     </row>
     <row r="115">
@@ -3641,7 +3641,7 @@
         <v>16</v>
       </c>
       <c r="H115" t="n">
-        <v>16.88712881926466</v>
+        <v>16.88714096449421</v>
       </c>
     </row>
     <row r="116">
@@ -3669,7 +3669,7 @@
         <v>13</v>
       </c>
       <c r="H116" t="n">
-        <v>14.27539080469169</v>
+        <v>14.27540356320856</v>
       </c>
     </row>
     <row r="117">
@@ -3697,7 +3697,7 @@
         <v>17</v>
       </c>
       <c r="H117" t="n">
-        <v>17.4523592393234</v>
+        <v>17.45236783218256</v>
       </c>
     </row>
     <row r="118">
@@ -3725,7 +3725,7 @@
         <v>16</v>
       </c>
       <c r="H118" t="n">
-        <v>16.00245916012561</v>
+        <v>16.00247061606213</v>
       </c>
     </row>
     <row r="119">
@@ -3753,7 +3753,7 @@
         <v>16</v>
       </c>
       <c r="H119" t="n">
-        <v>16.51693672736211</v>
+        <v>16.51692697571005</v>
       </c>
     </row>
     <row r="120">
@@ -3781,7 +3781,7 @@
         <v>15</v>
       </c>
       <c r="H120" t="n">
-        <v>14.89489329806758</v>
+        <v>14.89490011885211</v>
       </c>
     </row>
     <row r="121">
@@ -3809,7 +3809,7 @@
         <v>16</v>
       </c>
       <c r="H121" t="n">
-        <v>16.5134175068672</v>
+        <v>16.51342779579527</v>
       </c>
     </row>
     <row r="122">
@@ -3837,7 +3837,7 @@
         <v>17</v>
       </c>
       <c r="H122" t="n">
-        <v>16.80669683720571</v>
+        <v>16.8066995400477</v>
       </c>
     </row>
     <row r="123">
@@ -3865,7 +3865,7 @@
         <v>17</v>
       </c>
       <c r="H123" t="n">
-        <v>17.24727205652778</v>
+        <v>17.24728512430634</v>
       </c>
     </row>
     <row r="124">
@@ -3893,7 +3893,7 @@
         <v>18</v>
       </c>
       <c r="H124" t="n">
-        <v>18.87889690578017</v>
+        <v>18.8788432396263</v>
       </c>
     </row>
     <row r="125">
@@ -3945,7 +3945,7 @@
         <v>18</v>
       </c>
       <c r="H126" t="n">
-        <v>18.42522104600534</v>
+        <v>18.42522721699085</v>
       </c>
     </row>
     <row r="127">
@@ -3973,7 +3973,7 @@
         <v>15</v>
       </c>
       <c r="H127" t="n">
-        <v>15.70917982978711</v>
+        <v>15.70919887180971</v>
       </c>
     </row>
     <row r="128">
@@ -4001,7 +4001,7 @@
         <v>16</v>
       </c>
       <c r="H128" t="n">
-        <v>16.82632711180299</v>
+        <v>16.82630062748175</v>
       </c>
     </row>
     <row r="129">
@@ -4029,7 +4029,7 @@
         <v>17</v>
       </c>
       <c r="H129" t="n">
-        <v>17.62098336892524</v>
+        <v>17.62099829300529</v>
       </c>
     </row>
     <row r="130">
@@ -4057,7 +4057,7 @@
         <v>16</v>
       </c>
       <c r="H130" t="n">
-        <v>17.06181514832944</v>
+        <v>17.06180350386419</v>
       </c>
     </row>
     <row r="131">
@@ -4085,7 +4085,7 @@
         <v>15</v>
       </c>
       <c r="H131" t="n">
-        <v>15.05999820717451</v>
+        <v>15.06003139976007</v>
       </c>
     </row>
     <row r="132">
@@ -4113,7 +4113,7 @@
         <v>16</v>
       </c>
       <c r="H132" t="n">
-        <v>15.92855681221118</v>
+        <v>15.92859984067287</v>
       </c>
     </row>
     <row r="133">
@@ -4141,7 +4141,7 @@
         <v>16</v>
       </c>
       <c r="H133" t="n">
-        <v>15.27585596910368</v>
+        <v>15.27593318870846</v>
       </c>
     </row>
     <row r="134">
@@ -4169,7 +4169,7 @@
         <v>17</v>
       </c>
       <c r="H134" t="n">
-        <v>17.95725538660205</v>
+        <v>17.95729293336845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>